<commit_message>
Update API Posture Management Excel files
- Updated the API Posture Management - Concerns and Effectiveness Excel files to reflect the latest data and insights on API posture management.
</commit_message>
<xml_diff>
--- a/data/Section 3/3.2 API Posture Management/12 API Posture Management- Concern.xlsx
+++ b/data/Section 3/3.2 API Posture Management/12 API Posture Management- Concern.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft15392477-my.sharepoint.com/personal/nitin_acharekar_smartvalyou_ai/Documents/Survey Report/Section 3/API Posture Management/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft15392477-my.sharepoint.com/personal/nitin_acharekar_smartvalyou_ai/Documents/Survey Report/Survey Report Agent/surveyreport/data/Section 3/3.2 API Posture Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{FCEE8FE1-88B5-4D15-91BA-6858D787343D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64FA82FF-07D9-400B-820D-03179E49083A}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{FCEE8FE1-88B5-4D15-91BA-6858D787343D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D3C0C1F-209E-499F-8203-4BD99AF4A034}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EA068FB9-79C8-4995-ACCA-4A9D2E5A6387}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4020" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4022" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Extremely Concerning </t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -262,6 +268,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{346B9CC8-FB33-4039-A869-AB124BF695E7}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{346B9CC8-FB33-4039-A869-AB124BF695E7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{2A70E196-B8B2-416D-A58A-132D58E70537}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{22AB79FD-E110-43DB-A88A-04E77FC29DAF}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44650,10 +44667,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2321A4B-25AB-4034-8DFC-7BFCD5DC5B42}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44663,54 +44680,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>